<commit_message>
WIP adding more test cases for AStarSolver
</commit_message>
<xml_diff>
--- a/csharp_pathfinding/AStarTests/Resources/excel_mazes/spiral_hole1.xlsx
+++ b/csharp_pathfinding/AStarTests/Resources/excel_mazes/spiral_hole1.xlsx
@@ -206,329 +206,329 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
+      <selection pane="topLeft" activeCell="U8" activeCellId="0" sqref="U8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="36" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.5078125" defaultRowHeight="36" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -542,7 +542,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>